<commit_message>
#1376 - fixed issue for formula values and added additional testing coverage
</commit_message>
<xml_diff>
--- a/bundle/src/test/resources/com/adobe/acs/commons/data/spreadsheet-data-types.xlsx
+++ b/bundle/src/test/resources/com/adobe/acs/commons/data/spreadsheet-data-types.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brobert\Documents\Code Projects\acs-aem-commons\bundle\src\test\resources\com\adobe\acs\commons\mcp\impl\processes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brobert\Documents\Code Projects\acs-aem-commons\bundle\src\test\resources\com\adobe\acs\commons\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAD96BD-17CB-4CB2-A7C3-6FCAB9CB1CB4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26818CEC-00B8-4AED-9CCC-FB85FACC181A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{B989199F-66C5-4B28-BA4B-596AA9AB6E6A}"/>
   </bookViews>
@@ -62,8 +62,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -105,8 +105,8 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10CA0BE4-5450-449C-8A19-0FD38AB72831}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -502,6 +502,44 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <f>IF(ISBLANK(A2),"",A2)</f>
+        <v>123</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:I3" si="0">IF(ISBLANK(B2),"",B2)</f>
+        <v>123</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>123.456</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>123.456</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" si="0"/>
+        <v>31377</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" si="0"/>
+        <v>31377</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" si="0"/>
+        <v>0.375</v>
+      </c>
+      <c r="H3" s="5">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" si="0"/>
+        <v>This is just a regular string</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added additional date conversion test cases
</commit_message>
<xml_diff>
--- a/bundle/src/test/resources/com/adobe/acs/commons/data/spreadsheet-data-types.xlsx
+++ b/bundle/src/test/resources/com/adobe/acs/commons/data/spreadsheet-data-types.xlsx
@@ -1,31 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brobert\Documents\Code Projects\acs-aem-commons\bundle\src\test\resources\com\adobe\acs\commons\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brobert\Documents\code\acs-commons\bundle\src\test\resources\com\adobe\acs\commons\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26818CEC-00B8-4AED-9CCC-FB85FACC181A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B14449-1BE3-4799-829D-611F32AAD5F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{B989199F-66C5-4B28-BA4B-596AA9AB6E6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Integer</t>
   </si>
@@ -55,15 +60,32 @@
   </si>
   <si>
     <t>This is just a regular string</t>
+  </si>
+  <si>
+    <t>date1@date</t>
+  </si>
+  <si>
+    <t>date2@date</t>
+  </si>
+  <si>
+    <t>date3@date</t>
+  </si>
+  <si>
+    <t>date4@date</t>
+  </si>
+  <si>
+    <t>2000-01-01T14:47:41.922-05:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="169" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -102,13 +124,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10CA0BE4-5450-449C-8A19-0FD38AB72831}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -440,9 +467,13 @@
     <col min="7" max="7" width="10.73046875" customWidth="1"/>
     <col min="8" max="8" width="10.53125" customWidth="1"/>
     <col min="9" max="9" width="21.46484375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -470,8 +501,20 @@
       <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>123</v>
       </c>
@@ -501,8 +544,20 @@
       <c r="I2" t="s">
         <v>9</v>
       </c>
+      <c r="J2" s="10">
+        <v>36526</v>
+      </c>
+      <c r="K2" s="8">
+        <v>36526</v>
+      </c>
+      <c r="L2" s="7">
+        <v>36526</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3">
         <f>IF(ISBLANK(A2),"",A2)</f>
         <v>123</v>
@@ -538,6 +593,18 @@
       <c r="I3" t="str">
         <f t="shared" si="0"/>
         <v>This is just a regular string</v>
+      </c>
+      <c r="J3" s="10">
+        <v>36527</v>
+      </c>
+      <c r="K3" s="8">
+        <v>36526</v>
+      </c>
+      <c r="L3" s="7">
+        <v>36526</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected date handling as well as debugged and fixed affected issues in Date Importer tool.
</commit_message>
<xml_diff>
--- a/bundle/src/test/resources/com/adobe/acs/commons/data/spreadsheet-data-types.xlsx
+++ b/bundle/src/test/resources/com/adobe/acs/commons/data/spreadsheet-data-types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brobert\Documents\code\acs-commons\bundle\src\test\resources\com\adobe\acs\commons\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B14449-1BE3-4799-829D-611F32AAD5F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A81092F-490A-4635-A7C5-9C268E6DD08B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{B989199F-66C5-4B28-BA4B-596AA9AB6E6A}"/>
   </bookViews>
@@ -85,7 +85,7 @@
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="166" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="169" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -135,7 +135,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,7 +453,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J3"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -595,7 +595,7 @@
         <v>This is just a regular string</v>
       </c>
       <c r="J3" s="10">
-        <v>36527</v>
+        <v>36526</v>
       </c>
       <c r="K3" s="8">
         <v>36526</v>

</xml_diff>